<commit_message>
A bunch of improvements at the Lake:
* Calculating and logging power available at panel when throttled by
controller. Same as for Arduino-LCD. Determined it was PWM (Pulse Width
Modulation) kicking in when more power is available at the panel than
required to charge the battery.
* Power usage chart broken down much more: batter in/out, etc...
* Power usage chart has date range selection.
* Fliped LCD display to accomodate mounting orientation.
* Attempt at logging crashes.
* Fixed sensor read period logic to actually work.
* Rough calibration for solar system at the Lake.
</commit_message>
<xml_diff>
--- a/esp32-micropython/hardware/bom.xlsx
+++ b/esp32-micropython/hardware/bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clee\code\personal\power-meter\esp32-micropython\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A08ECD9-015D-4B07-A94F-317D7732BEC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5BBF6D-DDBB-4B12-B768-CF6D59EF49A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>ADS1115 16-Bit ADC - 4 Channel with Programmable Gain Amplifier</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1085</t>
+  </si>
+  <si>
+    <t>Canaduino</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/gp/product/B07BJF8JVK/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -90,7 +105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -129,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -445,15 +460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625"/>
     <col min="3" max="3" width="11.5703125"/>
     <col min="4" max="4" width="11.7109375"/>
@@ -554,6 +569,31 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
+      <c r="F7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>